<commit_message>
fix bulk uplaod fix
</commit_message>
<xml_diff>
--- a/public/Student-Bulk-Import-Sample.xlsx
+++ b/public/Student-Bulk-Import-Sample.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Students ID</t>
   </si>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Student Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Gender</t>
+    <t xml:space="preserve">Roll</t>
   </si>
   <si>
     <t xml:space="preserve">Father's Name</t>
@@ -91,16 +91,13 @@
     <t xml:space="preserve">Mobile (SMS)</t>
   </si>
   <si>
-    <t xml:space="preserve">mehedi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">khan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begum</t>
+    <t xml:space="preserve">sorna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anam</t>
   </si>
 </sst>
 </file>
@@ -233,7 +230,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,14 +289,14 @@
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>8801700000000</v>

</xml_diff>